<commit_message>
Updated code for reading (new)schedule
</commit_message>
<xml_diff>
--- a/Worksheet_Processing/OnCall_Tallies_Example_edited.xlsx
+++ b/Worksheet_Processing/OnCall_Tallies_Example_edited.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="101">
   <si>
     <t>St. John Paul II C.S.S.</t>
   </si>
@@ -390,6 +390,12 @@
   <si>
     <t>April</t>
   </si>
+  <si>
+    <t>RAG</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
 </sst>
 </file>
 
@@ -596,7 +602,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -869,11 +875,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1119,6 +1149,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1876,9 +1915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y116" sqref="Y116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1904,27 +1943,27 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="101"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="104"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="3"/>
       <c r="AC1" s="5"/>
@@ -1943,27 +1982,27 @@
       <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="104"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="107"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="3" t="s">
         <v>1</v>
@@ -1981,34 +2020,34 @@
       <c r="AM2" s="6"/>
     </row>
     <row r="3" spans="1:39" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="113"/>
-      <c r="Y3" s="115" t="s">
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111"/>
+      <c r="S3" s="111"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="112"/>
+      <c r="X3" s="116"/>
+      <c r="Y3" s="118" t="s">
         <v>3</v>
       </c>
       <c r="AA3" t="s">
@@ -2027,37 +2066,37 @@
       <c r="AM3" s="6"/>
     </row>
     <row r="4" spans="1:39" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="106"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="111"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="116"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="115"/>
+      <c r="X4" s="117"/>
+      <c r="Y4" s="119"/>
       <c r="AA4" t="s">
         <v>74</v>
       </c>
       <c r="AC4" s="8"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B5" s="106"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
@@ -2128,7 +2167,7 @@
       </c>
     </row>
     <row r="6" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="106"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="14">
         <v>1</v>
       </c>
@@ -2233,8 +2272,8 @@
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>16</v>
+      <c r="B8" s="101" t="s">
+        <v>37</v>
       </c>
       <c r="W8" s="35"/>
       <c r="Y8" s="38">
@@ -2250,8 +2289,8 @@
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>17</v>
+      <c r="B9" s="101" t="s">
+        <v>99</v>
       </c>
       <c r="W9" s="35"/>
       <c r="Y9" s="38">
@@ -2267,8 +2306,8 @@
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" s="42" t="s">
-        <v>18</v>
+      <c r="B10" s="101" t="s">
+        <v>59</v>
       </c>
       <c r="W10" s="35"/>
       <c r="Y10" s="38">
@@ -2284,8 +2323,8 @@
       <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>19</v>
+      <c r="B11" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="W11" s="35"/>
       <c r="Y11" s="38">
@@ -2301,13 +2340,16 @@
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" s="42" t="s">
-        <v>20</v>
+      <c r="B12" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="35">
+        <v>1</v>
       </c>
       <c r="W12" s="35"/>
       <c r="Y12" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA12" s="39"/>
       <c r="AB12" s="31"/>
@@ -2318,8 +2360,8 @@
       <c r="A13">
         <v>6</v>
       </c>
-      <c r="B13" s="42" t="s">
-        <v>21</v>
+      <c r="B13" s="101" t="s">
+        <v>100</v>
       </c>
       <c r="W13" s="35"/>
       <c r="Y13" s="38">
@@ -2335,8 +2377,8 @@
       <c r="A14">
         <v>7</v>
       </c>
-      <c r="B14" s="42" t="s">
-        <v>22</v>
+      <c r="B14" s="101" t="s">
+        <v>40</v>
       </c>
       <c r="W14" s="35"/>
       <c r="Y14" s="38">
@@ -2352,8 +2394,8 @@
       <c r="A15">
         <v>8</v>
       </c>
-      <c r="B15" s="42" t="s">
-        <v>23</v>
+      <c r="B15" s="101" t="s">
+        <v>16</v>
       </c>
       <c r="W15" s="35"/>
       <c r="Y15" s="38">
@@ -2369,9 +2411,7 @@
       <c r="A16">
         <v>9</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>24</v>
-      </c>
+      <c r="B16" s="101"/>
       <c r="W16" s="35"/>
       <c r="Y16" s="38">
         <f t="shared" si="0"/>
@@ -2386,9 +2426,7 @@
       <c r="A17">
         <v>10</v>
       </c>
-      <c r="B17" s="42" t="s">
-        <v>25</v>
-      </c>
+      <c r="B17" s="42"/>
       <c r="W17" s="35"/>
       <c r="Y17" s="38">
         <f t="shared" si="0"/>
@@ -2403,9 +2441,7 @@
       <c r="A18">
         <v>11</v>
       </c>
-      <c r="B18" s="42" t="s">
-        <v>26</v>
-      </c>
+      <c r="B18" s="42"/>
       <c r="W18" s="35"/>
       <c r="Y18" s="38">
         <f t="shared" si="0"/>
@@ -2420,9 +2456,7 @@
       <c r="A19">
         <v>12</v>
       </c>
-      <c r="B19" s="42" t="s">
-        <v>27</v>
-      </c>
+      <c r="B19" s="42"/>
       <c r="W19" s="35"/>
       <c r="Y19" s="38">
         <f t="shared" si="0"/>
@@ -2437,9 +2471,7 @@
       <c r="A20">
         <v>13</v>
       </c>
-      <c r="B20" s="42" t="s">
-        <v>28</v>
-      </c>
+      <c r="B20" s="42"/>
       <c r="W20" s="35"/>
       <c r="Y20" s="38">
         <f t="shared" si="0"/>
@@ -2454,9 +2486,7 @@
       <c r="A21">
         <v>14</v>
       </c>
-      <c r="B21" s="42" t="s">
-        <v>29</v>
-      </c>
+      <c r="B21" s="42"/>
       <c r="W21" s="35"/>
       <c r="Y21" s="38">
         <f t="shared" si="0"/>
@@ -2471,9 +2501,7 @@
       <c r="A22">
         <v>15</v>
       </c>
-      <c r="B22" s="42" t="s">
-        <v>30</v>
-      </c>
+      <c r="B22" s="42"/>
       <c r="W22" s="35"/>
       <c r="Y22" s="38">
         <f t="shared" si="0"/>
@@ -2488,9 +2516,7 @@
       <c r="A23">
         <v>16</v>
       </c>
-      <c r="B23" s="42" t="s">
-        <v>31</v>
-      </c>
+      <c r="B23" s="42"/>
       <c r="W23" s="35"/>
       <c r="Y23" s="38">
         <f t="shared" si="0"/>
@@ -2505,9 +2531,7 @@
       <c r="A24">
         <v>17</v>
       </c>
-      <c r="B24" s="42" t="s">
-        <v>32</v>
-      </c>
+      <c r="B24" s="42"/>
       <c r="W24" s="35"/>
       <c r="Y24" s="38">
         <f t="shared" si="0"/>
@@ -2522,9 +2546,7 @@
       <c r="A25">
         <v>18</v>
       </c>
-      <c r="B25" s="42" t="s">
-        <v>33</v>
-      </c>
+      <c r="B25" s="42"/>
       <c r="W25" s="35"/>
       <c r="Y25" s="38">
         <f t="shared" si="0"/>
@@ -2539,9 +2561,7 @@
       <c r="A26">
         <v>19</v>
       </c>
-      <c r="B26" s="42" t="s">
-        <v>34</v>
-      </c>
+      <c r="B26" s="42"/>
       <c r="W26" s="35"/>
       <c r="Y26" s="38">
         <f t="shared" si="0"/>
@@ -2556,9 +2576,7 @@
       <c r="A27">
         <v>20</v>
       </c>
-      <c r="B27" s="42" t="s">
-        <v>35</v>
-      </c>
+      <c r="B27" s="42"/>
       <c r="W27" s="35"/>
       <c r="Y27" s="38">
         <f t="shared" si="0"/>
@@ -2657,13 +2675,16 @@
       <c r="A34">
         <v>1</v>
       </c>
-      <c r="B34" s="60" t="s">
-        <v>36</v>
+      <c r="B34" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="36">
+        <v>1</v>
       </c>
       <c r="W34" s="35"/>
       <c r="Y34" s="38">
         <f t="shared" ref="Y34:Y57" si="1">SUM(C34:W34)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA34" s="39"/>
       <c r="AB34" s="31"/>
@@ -2674,13 +2695,16 @@
       <c r="A35">
         <v>2</v>
       </c>
-      <c r="B35" s="42" t="s">
-        <v>37</v>
+      <c r="B35" s="101" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="36">
+        <v>1</v>
       </c>
       <c r="W35" s="35"/>
       <c r="Y35" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA35" s="39"/>
       <c r="AB35" s="31"/>
@@ -2691,8 +2715,8 @@
       <c r="A36">
         <v>3</v>
       </c>
-      <c r="B36" s="42" t="s">
-        <v>38</v>
+      <c r="B36" s="101" t="s">
+        <v>59</v>
       </c>
       <c r="W36" s="35"/>
       <c r="Y36" s="38">
@@ -2708,13 +2732,16 @@
       <c r="A37">
         <v>4</v>
       </c>
-      <c r="B37" s="42" t="s">
-        <v>39</v>
+      <c r="B37" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" s="36">
+        <v>1</v>
       </c>
       <c r="W37" s="35"/>
       <c r="Y37" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA37" s="39"/>
       <c r="AB37" s="31"/>
@@ -2725,13 +2752,16 @@
       <c r="A38">
         <v>5</v>
       </c>
-      <c r="B38" s="42" t="s">
-        <v>40</v>
+      <c r="B38" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="36">
+        <v>1</v>
       </c>
       <c r="W38" s="35"/>
       <c r="Y38" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA38" s="39"/>
       <c r="AB38" s="31"/>
@@ -2742,13 +2772,16 @@
       <c r="A39">
         <v>6</v>
       </c>
-      <c r="B39" s="42" t="s">
-        <v>41</v>
+      <c r="B39" s="101" t="s">
+        <v>100</v>
+      </c>
+      <c r="F39" s="36">
+        <v>1</v>
       </c>
       <c r="W39" s="35"/>
       <c r="Y39" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA39" s="39"/>
       <c r="AB39" s="31"/>
@@ -2759,13 +2792,16 @@
       <c r="A40">
         <v>7</v>
       </c>
-      <c r="B40" s="42" t="s">
-        <v>42</v>
+      <c r="B40" s="101" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="36">
+        <v>1</v>
       </c>
       <c r="W40" s="35"/>
       <c r="Y40" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA40" s="39"/>
       <c r="AB40" s="31"/>
@@ -2776,13 +2812,16 @@
       <c r="A41">
         <v>8</v>
       </c>
-      <c r="B41" s="42" t="s">
-        <v>43</v>
+      <c r="B41" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="36">
+        <v>1</v>
       </c>
       <c r="W41" s="35"/>
       <c r="Y41" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA41" s="39"/>
       <c r="AB41" s="31"/>
@@ -2793,9 +2832,7 @@
       <c r="A42">
         <v>9</v>
       </c>
-      <c r="B42" s="42" t="s">
-        <v>44</v>
-      </c>
+      <c r="B42" s="101"/>
       <c r="W42" s="35"/>
       <c r="Y42" s="38">
         <f t="shared" si="1"/>
@@ -2810,9 +2847,7 @@
       <c r="A43">
         <v>10</v>
       </c>
-      <c r="B43" s="42" t="s">
-        <v>45</v>
-      </c>
+      <c r="B43" s="42"/>
       <c r="W43" s="35"/>
       <c r="Y43" s="38">
         <f t="shared" si="1"/>
@@ -2827,9 +2862,7 @@
       <c r="A44">
         <v>11</v>
       </c>
-      <c r="B44" s="42" t="s">
-        <v>46</v>
-      </c>
+      <c r="B44" s="42"/>
       <c r="W44" s="35"/>
       <c r="Y44" s="38">
         <f t="shared" si="1"/>
@@ -2844,9 +2877,7 @@
       <c r="A45">
         <v>12</v>
       </c>
-      <c r="B45" s="42" t="s">
-        <v>47</v>
-      </c>
+      <c r="B45" s="42"/>
       <c r="W45" s="35"/>
       <c r="Y45" s="38">
         <f t="shared" si="1"/>
@@ -2861,9 +2892,7 @@
       <c r="A46">
         <v>13</v>
       </c>
-      <c r="B46" s="42" t="s">
-        <v>29</v>
-      </c>
+      <c r="B46" s="42"/>
       <c r="W46" s="35"/>
       <c r="Y46" s="38">
         <f t="shared" si="1"/>
@@ -2878,9 +2907,7 @@
       <c r="A47">
         <v>14</v>
       </c>
-      <c r="B47" s="42" t="s">
-        <v>48</v>
-      </c>
+      <c r="B47" s="42"/>
       <c r="W47" s="35"/>
       <c r="Y47" s="38">
         <f t="shared" si="1"/>
@@ -2895,9 +2922,7 @@
       <c r="A48">
         <v>15</v>
       </c>
-      <c r="B48" s="42" t="s">
-        <v>47</v>
-      </c>
+      <c r="B48" s="42"/>
       <c r="W48" s="35"/>
       <c r="Y48" s="38">
         <f t="shared" si="1"/>
@@ -2912,9 +2937,7 @@
       <c r="A49">
         <v>16</v>
       </c>
-      <c r="B49" s="60" t="s">
-        <v>49</v>
-      </c>
+      <c r="B49" s="60"/>
       <c r="W49" s="35"/>
       <c r="Y49" s="38">
         <f t="shared" si="1"/>
@@ -2929,9 +2952,7 @@
       <c r="A50">
         <v>17</v>
       </c>
-      <c r="B50" s="60" t="s">
-        <v>50</v>
-      </c>
+      <c r="B50" s="60"/>
       <c r="W50" s="35"/>
       <c r="Y50" s="38">
         <f t="shared" si="1"/>
@@ -2946,9 +2967,7 @@
       <c r="A51">
         <v>18</v>
       </c>
-      <c r="B51" s="60" t="s">
-        <v>51</v>
-      </c>
+      <c r="B51" s="60"/>
       <c r="W51" s="35"/>
       <c r="Y51" s="38">
         <f t="shared" si="1"/>
@@ -2963,9 +2982,7 @@
       <c r="A52">
         <v>19</v>
       </c>
-      <c r="B52" s="60" t="s">
-        <v>52</v>
-      </c>
+      <c r="B52" s="60"/>
       <c r="W52" s="35"/>
       <c r="Y52" s="38">
         <f t="shared" si="1"/>
@@ -2980,9 +2997,7 @@
       <c r="A53">
         <v>20</v>
       </c>
-      <c r="B53" s="60" t="s">
-        <v>53</v>
-      </c>
+      <c r="B53" s="60"/>
       <c r="W53" s="35"/>
       <c r="Y53" s="38">
         <f t="shared" si="1"/>
@@ -2997,9 +3012,7 @@
       <c r="A54">
         <v>21</v>
       </c>
-      <c r="B54" s="60" t="s">
-        <v>54</v>
-      </c>
+      <c r="B54" s="60"/>
       <c r="W54" s="35"/>
       <c r="Y54" s="38">
         <f t="shared" si="1"/>
@@ -3014,9 +3027,7 @@
       <c r="A55">
         <v>22</v>
       </c>
-      <c r="B55" s="60" t="s">
-        <v>55</v>
-      </c>
+      <c r="B55" s="60"/>
       <c r="W55" s="35"/>
       <c r="Y55" s="38">
         <f t="shared" si="1"/>
@@ -3031,9 +3042,7 @@
       <c r="A56">
         <v>23</v>
       </c>
-      <c r="B56" s="61" t="s">
-        <v>56</v>
-      </c>
+      <c r="B56" s="61"/>
       <c r="W56" s="35"/>
       <c r="Y56" s="38">
         <f t="shared" si="1"/>
@@ -3048,9 +3057,7 @@
       <c r="A57">
         <v>24</v>
       </c>
-      <c r="B57" s="34" t="s">
-        <v>57</v>
-      </c>
+      <c r="B57" s="34"/>
       <c r="W57" s="35"/>
       <c r="Y57" s="38">
         <f t="shared" si="1"/>
@@ -3109,8 +3116,8 @@
       <c r="A60">
         <v>1</v>
       </c>
-      <c r="B60" s="42" t="s">
-        <v>75</v>
+      <c r="B60" s="101" t="s">
+        <v>37</v>
       </c>
       <c r="W60" s="35"/>
       <c r="Y60" s="38">
@@ -3126,8 +3133,8 @@
       <c r="A61">
         <v>2</v>
       </c>
-      <c r="B61" s="42" t="s">
-        <v>76</v>
+      <c r="B61" s="101" t="s">
+        <v>99</v>
       </c>
       <c r="W61" s="35"/>
       <c r="Y61" s="38">
@@ -3143,8 +3150,8 @@
       <c r="A62">
         <v>3</v>
       </c>
-      <c r="B62" s="65" t="s">
-        <v>77</v>
+      <c r="B62" s="101" t="s">
+        <v>59</v>
       </c>
       <c r="W62" s="35"/>
       <c r="Y62" s="38">
@@ -3160,8 +3167,8 @@
       <c r="A63">
         <v>4</v>
       </c>
-      <c r="B63" s="60" t="s">
-        <v>78</v>
+      <c r="B63" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="W63" s="35"/>
       <c r="Y63" s="38">
@@ -3177,8 +3184,8 @@
       <c r="A64">
         <v>5</v>
       </c>
-      <c r="B64" s="60" t="s">
-        <v>79</v>
+      <c r="B64" s="101" t="s">
+        <v>41</v>
       </c>
       <c r="W64" s="35"/>
       <c r="Y64" s="38">
@@ -3194,8 +3201,8 @@
       <c r="A65">
         <v>6</v>
       </c>
-      <c r="B65" s="60" t="s">
-        <v>80</v>
+      <c r="B65" s="101" t="s">
+        <v>100</v>
       </c>
       <c r="W65" s="35"/>
       <c r="Y65" s="38">
@@ -3211,8 +3218,8 @@
       <c r="A66">
         <v>7</v>
       </c>
-      <c r="B66" s="60" t="s">
-        <v>81</v>
+      <c r="B66" s="101" t="s">
+        <v>40</v>
       </c>
       <c r="W66" s="35"/>
       <c r="Y66" s="38">
@@ -3228,8 +3235,8 @@
       <c r="A67">
         <v>8</v>
       </c>
-      <c r="B67" s="60" t="s">
-        <v>82</v>
+      <c r="B67" s="101" t="s">
+        <v>16</v>
       </c>
       <c r="W67" s="35"/>
       <c r="Y67" s="38">
@@ -3245,9 +3252,7 @@
       <c r="A68">
         <v>9</v>
       </c>
-      <c r="B68" s="60" t="s">
-        <v>83</v>
-      </c>
+      <c r="B68" s="101"/>
       <c r="W68" s="35"/>
       <c r="Y68" s="38">
         <f t="shared" si="2"/>
@@ -3262,9 +3267,7 @@
       <c r="A69">
         <v>10</v>
       </c>
-      <c r="B69" s="42" t="s">
-        <v>84</v>
-      </c>
+      <c r="B69" s="42"/>
       <c r="W69" s="35"/>
       <c r="Y69" s="38">
         <f t="shared" si="2"/>
@@ -3279,9 +3282,7 @@
       <c r="A70">
         <v>11</v>
       </c>
-      <c r="B70" s="42" t="s">
-        <v>85</v>
-      </c>
+      <c r="B70" s="42"/>
       <c r="W70" s="35"/>
       <c r="Y70" s="38">
         <f t="shared" si="2"/>
@@ -3296,9 +3297,7 @@
       <c r="A71">
         <v>12</v>
       </c>
-      <c r="B71" s="42" t="s">
-        <v>86</v>
-      </c>
+      <c r="B71" s="42"/>
       <c r="W71" s="35"/>
       <c r="Y71" s="38">
         <f t="shared" si="2"/>
@@ -3313,9 +3312,7 @@
       <c r="A72">
         <v>13</v>
       </c>
-      <c r="B72" s="42" t="s">
-        <v>87</v>
-      </c>
+      <c r="B72" s="42"/>
       <c r="W72" s="35"/>
       <c r="Y72" s="38">
         <f t="shared" si="2"/>
@@ -3330,9 +3327,7 @@
       <c r="A73">
         <v>14</v>
       </c>
-      <c r="B73" s="42" t="s">
-        <v>88</v>
-      </c>
+      <c r="B73" s="42"/>
       <c r="W73" s="35"/>
       <c r="Y73" s="38">
         <f t="shared" si="2"/>
@@ -3347,9 +3342,7 @@
       <c r="A74">
         <v>15</v>
       </c>
-      <c r="B74" s="42" t="s">
-        <v>66</v>
-      </c>
+      <c r="B74" s="42"/>
       <c r="W74" s="35"/>
       <c r="Y74" s="38">
         <f t="shared" si="2"/>
@@ -3364,9 +3357,7 @@
       <c r="A75">
         <v>16</v>
       </c>
-      <c r="B75" s="42" t="s">
-        <v>89</v>
-      </c>
+      <c r="B75" s="42"/>
       <c r="W75" s="35"/>
       <c r="Y75" s="38">
         <f t="shared" si="2"/>
@@ -3381,9 +3372,7 @@
       <c r="A76">
         <v>17</v>
       </c>
-      <c r="B76" s="42" t="s">
-        <v>90</v>
-      </c>
+      <c r="B76" s="42"/>
       <c r="W76" s="35"/>
       <c r="Y76" s="38">
         <f t="shared" si="2"/>
@@ -3398,9 +3387,7 @@
       <c r="A77">
         <v>18</v>
       </c>
-      <c r="B77" s="42" t="s">
-        <v>89</v>
-      </c>
+      <c r="B77" s="42"/>
       <c r="W77" s="35"/>
       <c r="Y77" s="38">
         <f t="shared" si="2"/>
@@ -3415,9 +3402,7 @@
       <c r="A78">
         <v>19</v>
       </c>
-      <c r="B78" s="42" t="s">
-        <v>91</v>
-      </c>
+      <c r="B78" s="42"/>
       <c r="W78" s="35"/>
       <c r="Y78" s="38">
         <f t="shared" si="2"/>
@@ -3432,9 +3417,7 @@
       <c r="A79">
         <v>20</v>
       </c>
-      <c r="B79" s="42" t="s">
-        <v>92</v>
-      </c>
+      <c r="B79" s="42"/>
       <c r="W79" s="35"/>
       <c r="Y79" s="38">
         <f t="shared" si="2"/>
@@ -3449,9 +3432,7 @@
       <c r="A80">
         <v>21</v>
       </c>
-      <c r="B80" s="42" t="s">
-        <v>93</v>
-      </c>
+      <c r="B80" s="42"/>
       <c r="W80" s="35"/>
       <c r="Y80" s="38">
         <f t="shared" si="2"/>
@@ -3466,9 +3447,7 @@
       <c r="A81">
         <v>22</v>
       </c>
-      <c r="B81" s="42" t="s">
-        <v>94</v>
-      </c>
+      <c r="B81" s="42"/>
       <c r="W81" s="35"/>
       <c r="Y81" s="38">
         <f t="shared" si="2"/>
@@ -3483,9 +3462,7 @@
       <c r="A82">
         <v>23</v>
       </c>
-      <c r="B82" s="66" t="s">
-        <v>95</v>
-      </c>
+      <c r="B82" s="66"/>
       <c r="W82" s="35"/>
       <c r="Y82" s="38">
         <f t="shared" si="2"/>
@@ -3554,8 +3531,8 @@
       <c r="A86">
         <v>1</v>
       </c>
-      <c r="B86" s="60" t="s">
-        <v>58</v>
+      <c r="B86" s="101" t="s">
+        <v>37</v>
       </c>
       <c r="W86" s="35"/>
       <c r="Y86" s="38">
@@ -3571,8 +3548,8 @@
       <c r="A87">
         <v>2</v>
       </c>
-      <c r="B87" s="60" t="s">
-        <v>59</v>
+      <c r="B87" s="101" t="s">
+        <v>99</v>
       </c>
       <c r="W87" s="35"/>
       <c r="Y87" s="38">
@@ -3588,8 +3565,8 @@
       <c r="A88">
         <v>3</v>
       </c>
-      <c r="B88" s="60" t="s">
-        <v>60</v>
+      <c r="B88" s="101" t="s">
+        <v>59</v>
       </c>
       <c r="W88" s="35"/>
       <c r="Y88" s="38">
@@ -3605,8 +3582,8 @@
       <c r="A89">
         <v>4</v>
       </c>
-      <c r="B89" s="60" t="s">
-        <v>61</v>
+      <c r="B89" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="W89" s="35"/>
       <c r="Y89" s="38">
@@ -3622,8 +3599,8 @@
       <c r="A90">
         <v>5</v>
       </c>
-      <c r="B90" s="60" t="s">
-        <v>62</v>
+      <c r="B90" s="101" t="s">
+        <v>41</v>
       </c>
       <c r="W90" s="35"/>
       <c r="Y90" s="38">
@@ -3639,8 +3616,8 @@
       <c r="A91">
         <v>6</v>
       </c>
-      <c r="B91" s="60" t="s">
-        <v>45</v>
+      <c r="B91" s="101" t="s">
+        <v>100</v>
       </c>
       <c r="W91" s="35"/>
       <c r="Y91" s="38">
@@ -3656,8 +3633,8 @@
       <c r="A92">
         <v>7</v>
       </c>
-      <c r="B92" s="60" t="s">
-        <v>63</v>
+      <c r="B92" s="101" t="s">
+        <v>40</v>
       </c>
       <c r="W92" s="35"/>
       <c r="Y92" s="38">
@@ -3673,8 +3650,8 @@
       <c r="A93">
         <v>8</v>
       </c>
-      <c r="B93" s="60" t="s">
-        <v>64</v>
+      <c r="B93" s="101" t="s">
+        <v>16</v>
       </c>
       <c r="W93" s="35"/>
       <c r="Y93" s="38">
@@ -3690,9 +3667,7 @@
       <c r="A94">
         <v>9</v>
       </c>
-      <c r="B94" s="60" t="s">
-        <v>27</v>
-      </c>
+      <c r="B94" s="101"/>
       <c r="W94" s="35"/>
       <c r="Y94" s="38">
         <f t="shared" si="3"/>
@@ -3707,9 +3682,7 @@
       <c r="A95">
         <v>10</v>
       </c>
-      <c r="B95" s="60" t="s">
-        <v>65</v>
-      </c>
+      <c r="B95" s="60"/>
       <c r="W95" s="35"/>
       <c r="Y95" s="38">
         <f t="shared" si="3"/>
@@ -3724,9 +3697,7 @@
       <c r="A96">
         <v>11</v>
       </c>
-      <c r="B96" s="60" t="s">
-        <v>29</v>
-      </c>
+      <c r="B96" s="60"/>
       <c r="W96" s="35"/>
       <c r="Y96" s="38">
         <f t="shared" si="3"/>
@@ -3741,9 +3712,7 @@
       <c r="A97">
         <v>12</v>
       </c>
-      <c r="B97" s="60" t="s">
-        <v>66</v>
-      </c>
+      <c r="B97" s="60"/>
       <c r="W97" s="35"/>
       <c r="Y97" s="38">
         <f t="shared" si="3"/>
@@ -3758,9 +3727,7 @@
       <c r="A98">
         <v>13</v>
       </c>
-      <c r="B98" s="60" t="s">
-        <v>67</v>
-      </c>
+      <c r="B98" s="60"/>
       <c r="W98" s="35"/>
       <c r="Y98" s="38">
         <f t="shared" si="3"/>
@@ -3775,9 +3742,7 @@
       <c r="A99">
         <v>14</v>
       </c>
-      <c r="B99" s="60" t="s">
-        <v>47</v>
-      </c>
+      <c r="B99" s="60"/>
       <c r="W99" s="35"/>
       <c r="Y99" s="38">
         <f t="shared" si="3"/>
@@ -3792,9 +3757,7 @@
       <c r="A100">
         <v>15</v>
       </c>
-      <c r="B100" s="60" t="s">
-        <v>68</v>
-      </c>
+      <c r="B100" s="60"/>
       <c r="W100" s="35"/>
       <c r="Y100" s="38">
         <f t="shared" si="3"/>
@@ -3809,9 +3772,7 @@
       <c r="A101">
         <v>16</v>
       </c>
-      <c r="B101" s="60" t="s">
-        <v>69</v>
-      </c>
+      <c r="B101" s="60"/>
       <c r="W101" s="35"/>
       <c r="Y101" s="38">
         <f t="shared" si="3"/>
@@ -3826,9 +3787,7 @@
       <c r="A102">
         <v>17</v>
       </c>
-      <c r="B102" s="60" t="s">
-        <v>70</v>
-      </c>
+      <c r="B102" s="60"/>
       <c r="W102" s="35"/>
       <c r="Y102" s="38">
         <f t="shared" si="3"/>
@@ -3843,9 +3802,7 @@
       <c r="A103">
         <v>18</v>
       </c>
-      <c r="B103" s="60" t="s">
-        <v>71</v>
-      </c>
+      <c r="B103" s="60"/>
       <c r="W103" s="35"/>
       <c r="Y103" s="38">
         <f t="shared" si="3"/>
@@ -3860,9 +3817,7 @@
       <c r="A104">
         <v>19</v>
       </c>
-      <c r="B104" s="60" t="s">
-        <v>52</v>
-      </c>
+      <c r="B104" s="60"/>
       <c r="W104" s="35"/>
       <c r="Y104" s="38">
         <f t="shared" si="3"/>
@@ -3877,9 +3832,7 @@
       <c r="A105">
         <v>20</v>
       </c>
-      <c r="B105" s="60" t="s">
-        <v>72</v>
-      </c>
+      <c r="B105" s="60"/>
       <c r="W105" s="35"/>
       <c r="Y105" s="38">
         <f t="shared" si="3"/>
@@ -3961,7 +3914,7 @@
       <c r="X111" s="74"/>
       <c r="Y111" s="75">
         <f>SUM(Y8:Y105)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:30" x14ac:dyDescent="0.2">
@@ -6672,27 +6625,27 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="101"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="104"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="3"/>
       <c r="AB1" s="4"/>
@@ -6702,27 +6655,27 @@
       <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="104"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="107"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="3" t="s">
         <v>1</v>
@@ -6731,34 +6684,34 @@
       <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" ht="24" x14ac:dyDescent="0.2">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="110" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="113"/>
-      <c r="Y3" s="115" t="s">
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111"/>
+      <c r="S3" s="111"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="112"/>
+      <c r="X3" s="116"/>
+      <c r="Y3" s="118" t="s">
         <v>3</v>
       </c>
       <c r="AA3" t="s">
@@ -6768,30 +6721,30 @@
       <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B4" s="106"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="111"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="116"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="115"/>
+      <c r="X4" s="117"/>
+      <c r="Y4" s="119"/>
       <c r="AA4" t="s">
         <v>74</v>
       </c>
@@ -6799,7 +6752,7 @@
       <c r="AC4" s="8"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B5" s="106"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
@@ -6872,7 +6825,7 @@
       <c r="AC5" s="13"/>
     </row>
     <row r="6" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="106"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="14">
         <v>1</v>
       </c>
@@ -10865,27 +10818,27 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="101"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="104"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="3"/>
       <c r="AB1" s="4"/>
@@ -10895,27 +10848,27 @@
       <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="104"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="107"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="3" t="s">
         <v>1</v>
@@ -10924,34 +10877,34 @@
       <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" ht="24" x14ac:dyDescent="0.2">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="113"/>
-      <c r="Y3" s="115" t="s">
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111"/>
+      <c r="S3" s="111"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="112"/>
+      <c r="X3" s="116"/>
+      <c r="Y3" s="118" t="s">
         <v>3</v>
       </c>
       <c r="AA3" t="s">
@@ -10961,30 +10914,30 @@
       <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B4" s="106"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="111"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="116"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="115"/>
+      <c r="X4" s="117"/>
+      <c r="Y4" s="119"/>
       <c r="AA4" t="s">
         <v>74</v>
       </c>
@@ -10992,7 +10945,7 @@
       <c r="AC4" s="8"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B5" s="106"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
@@ -11067,7 +11020,7 @@
       <c r="AC5" s="13"/>
     </row>
     <row r="6" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="106"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="14">
         <v>1</v>
       </c>
@@ -15022,8 +14975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:W117"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95:B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15032,27 +14985,27 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="101"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="104"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="3"/>
       <c r="AB1" s="4"/>
@@ -15062,27 +15015,27 @@
       <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="104"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="107"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="3" t="s">
         <v>1</v>
@@ -15091,34 +15044,34 @@
       <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" ht="24" x14ac:dyDescent="0.2">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="110" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="113"/>
-      <c r="Y3" s="115" t="s">
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111"/>
+      <c r="S3" s="111"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="112"/>
+      <c r="X3" s="116"/>
+      <c r="Y3" s="118" t="s">
         <v>3</v>
       </c>
       <c r="AA3" t="s">
@@ -15128,30 +15081,30 @@
       <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B4" s="106"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="111"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="116"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="115"/>
+      <c r="X4" s="117"/>
+      <c r="Y4" s="119"/>
       <c r="AA4" t="s">
         <v>74</v>
       </c>
@@ -15159,7 +15112,7 @@
       <c r="AC4" s="8"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B5" s="106"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
@@ -15232,7 +15185,7 @@
       <c r="AC5" s="13"/>
     </row>
     <row r="6" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="106"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="14">
         <v>1</v>
       </c>
@@ -15336,8 +15289,8 @@
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>16</v>
+      <c r="B8" s="99" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="36"/>
@@ -15373,8 +15326,8 @@
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>17</v>
+      <c r="B9" s="100" t="s">
+        <v>99</v>
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="36"/>
@@ -15410,8 +15363,8 @@
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" s="42" t="s">
-        <v>18</v>
+      <c r="B10" s="100" t="s">
+        <v>59</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
@@ -15447,8 +15400,8 @@
       <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>19</v>
+      <c r="B11" s="100" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="36"/>
@@ -15484,8 +15437,8 @@
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" s="42" t="s">
-        <v>20</v>
+      <c r="B12" s="100" t="s">
+        <v>41</v>
       </c>
       <c r="C12" s="35"/>
       <c r="D12" s="36"/>
@@ -15521,8 +15474,8 @@
       <c r="A13">
         <v>6</v>
       </c>
-      <c r="B13" s="42" t="s">
-        <v>21</v>
+      <c r="B13" s="100" t="s">
+        <v>100</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="36"/>
@@ -15558,8 +15511,8 @@
       <c r="A14">
         <v>7</v>
       </c>
-      <c r="B14" s="42" t="s">
-        <v>22</v>
+      <c r="B14" s="100" t="s">
+        <v>38</v>
       </c>
       <c r="C14" s="35"/>
       <c r="D14" s="36"/>
@@ -15595,8 +15548,8 @@
       <c r="A15">
         <v>8</v>
       </c>
-      <c r="B15" s="42" t="s">
-        <v>23</v>
+      <c r="B15" s="100" t="s">
+        <v>40</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
@@ -15632,8 +15585,8 @@
       <c r="A16">
         <v>9</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>24</v>
+      <c r="B16" s="100" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
@@ -15669,9 +15622,7 @@
       <c r="A17">
         <v>10</v>
       </c>
-      <c r="B17" s="42" t="s">
-        <v>25</v>
-      </c>
+      <c r="B17" s="42"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
       <c r="E17" s="36"/>
@@ -15706,9 +15657,7 @@
       <c r="A18">
         <v>11</v>
       </c>
-      <c r="B18" s="42" t="s">
-        <v>26</v>
-      </c>
+      <c r="B18" s="42"/>
       <c r="C18" s="35"/>
       <c r="D18" s="36"/>
       <c r="E18" s="36"/>
@@ -15743,9 +15692,7 @@
       <c r="A19">
         <v>12</v>
       </c>
-      <c r="B19" s="42" t="s">
-        <v>27</v>
-      </c>
+      <c r="B19" s="42"/>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
       <c r="E19" s="36"/>
@@ -15780,9 +15727,7 @@
       <c r="A20">
         <v>13</v>
       </c>
-      <c r="B20" s="42" t="s">
-        <v>28</v>
-      </c>
+      <c r="B20" s="42"/>
       <c r="C20" s="35"/>
       <c r="D20" s="36"/>
       <c r="E20" s="36"/>
@@ -15817,9 +15762,7 @@
       <c r="A21">
         <v>14</v>
       </c>
-      <c r="B21" s="42" t="s">
-        <v>29</v>
-      </c>
+      <c r="B21" s="42"/>
       <c r="C21" s="35"/>
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
@@ -15854,9 +15797,7 @@
       <c r="A22">
         <v>15</v>
       </c>
-      <c r="B22" s="42" t="s">
-        <v>30</v>
-      </c>
+      <c r="B22" s="42"/>
       <c r="C22" s="35"/>
       <c r="D22" s="36"/>
       <c r="E22" s="36"/>
@@ -15891,9 +15832,7 @@
       <c r="A23">
         <v>16</v>
       </c>
-      <c r="B23" s="42" t="s">
-        <v>31</v>
-      </c>
+      <c r="B23" s="42"/>
       <c r="C23" s="35"/>
       <c r="D23" s="36"/>
       <c r="E23" s="36"/>
@@ -15928,9 +15867,7 @@
       <c r="A24">
         <v>17</v>
       </c>
-      <c r="B24" s="42" t="s">
-        <v>32</v>
-      </c>
+      <c r="B24" s="42"/>
       <c r="C24" s="35"/>
       <c r="D24" s="36"/>
       <c r="E24" s="36"/>
@@ -15965,9 +15902,7 @@
       <c r="A25">
         <v>18</v>
       </c>
-      <c r="B25" s="42" t="s">
-        <v>33</v>
-      </c>
+      <c r="B25" s="42"/>
       <c r="C25" s="35"/>
       <c r="D25" s="36"/>
       <c r="E25" s="36"/>
@@ -16002,9 +15937,7 @@
       <c r="A26">
         <v>19</v>
       </c>
-      <c r="B26" s="42" t="s">
-        <v>34</v>
-      </c>
+      <c r="B26" s="42"/>
       <c r="C26" s="35"/>
       <c r="D26" s="36"/>
       <c r="E26" s="36"/>
@@ -16039,9 +15972,7 @@
       <c r="A27">
         <v>20</v>
       </c>
-      <c r="B27" s="42" t="s">
-        <v>35</v>
-      </c>
+      <c r="B27" s="42"/>
       <c r="C27" s="35"/>
       <c r="D27" s="36"/>
       <c r="E27" s="36"/>
@@ -16266,8 +16197,8 @@
       <c r="A34">
         <v>1</v>
       </c>
-      <c r="B34" s="60" t="s">
-        <v>36</v>
+      <c r="B34" s="101" t="s">
+        <v>37</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="36"/>
@@ -16303,8 +16234,8 @@
       <c r="A35">
         <v>2</v>
       </c>
-      <c r="B35" s="42" t="s">
-        <v>37</v>
+      <c r="B35" s="101" t="s">
+        <v>99</v>
       </c>
       <c r="C35" s="35"/>
       <c r="D35" s="36"/>
@@ -16340,8 +16271,8 @@
       <c r="A36">
         <v>3</v>
       </c>
-      <c r="B36" s="42" t="s">
-        <v>38</v>
+      <c r="B36" s="101" t="s">
+        <v>59</v>
       </c>
       <c r="C36" s="35"/>
       <c r="D36" s="36"/>
@@ -16377,8 +16308,8 @@
       <c r="A37">
         <v>4</v>
       </c>
-      <c r="B37" s="42" t="s">
-        <v>39</v>
+      <c r="B37" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
@@ -16414,8 +16345,8 @@
       <c r="A38">
         <v>5</v>
       </c>
-      <c r="B38" s="42" t="s">
-        <v>40</v>
+      <c r="B38" s="101" t="s">
+        <v>41</v>
       </c>
       <c r="C38" s="35"/>
       <c r="D38" s="36"/>
@@ -16451,8 +16382,8 @@
       <c r="A39">
         <v>6</v>
       </c>
-      <c r="B39" s="42" t="s">
-        <v>41</v>
+      <c r="B39" s="101" t="s">
+        <v>100</v>
       </c>
       <c r="C39" s="35"/>
       <c r="D39" s="36"/>
@@ -16488,8 +16419,8 @@
       <c r="A40">
         <v>7</v>
       </c>
-      <c r="B40" s="42" t="s">
-        <v>42</v>
+      <c r="B40" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="36"/>
@@ -16525,8 +16456,8 @@
       <c r="A41">
         <v>8</v>
       </c>
-      <c r="B41" s="42" t="s">
-        <v>43</v>
+      <c r="B41" s="101" t="s">
+        <v>40</v>
       </c>
       <c r="C41" s="35"/>
       <c r="D41" s="36"/>
@@ -16562,8 +16493,8 @@
       <c r="A42">
         <v>9</v>
       </c>
-      <c r="B42" s="42" t="s">
-        <v>44</v>
+      <c r="B42" s="101" t="s">
+        <v>16</v>
       </c>
       <c r="C42" s="35"/>
       <c r="D42" s="36"/>
@@ -16599,9 +16530,7 @@
       <c r="A43">
         <v>10</v>
       </c>
-      <c r="B43" s="42" t="s">
-        <v>45</v>
-      </c>
+      <c r="B43" s="42"/>
       <c r="C43" s="35"/>
       <c r="D43" s="36"/>
       <c r="E43" s="36"/>
@@ -16636,9 +16565,7 @@
       <c r="A44">
         <v>11</v>
       </c>
-      <c r="B44" s="42" t="s">
-        <v>46</v>
-      </c>
+      <c r="B44" s="42"/>
       <c r="C44" s="35"/>
       <c r="D44" s="36"/>
       <c r="E44" s="36"/>
@@ -16673,9 +16600,7 @@
       <c r="A45">
         <v>12</v>
       </c>
-      <c r="B45" s="42" t="s">
-        <v>47</v>
-      </c>
+      <c r="B45" s="42"/>
       <c r="C45" s="35"/>
       <c r="D45" s="36"/>
       <c r="E45" s="36"/>
@@ -16710,9 +16635,7 @@
       <c r="A46">
         <v>13</v>
       </c>
-      <c r="B46" s="42" t="s">
-        <v>29</v>
-      </c>
+      <c r="B46" s="42"/>
       <c r="C46" s="35"/>
       <c r="D46" s="36"/>
       <c r="E46" s="36"/>
@@ -16747,9 +16670,7 @@
       <c r="A47">
         <v>14</v>
       </c>
-      <c r="B47" s="42" t="s">
-        <v>48</v>
-      </c>
+      <c r="B47" s="42"/>
       <c r="C47" s="35"/>
       <c r="D47" s="36"/>
       <c r="E47" s="36"/>
@@ -16784,9 +16705,7 @@
       <c r="A48">
         <v>15</v>
       </c>
-      <c r="B48" s="42" t="s">
-        <v>47</v>
-      </c>
+      <c r="B48" s="42"/>
       <c r="C48" s="35"/>
       <c r="D48" s="36"/>
       <c r="E48" s="36"/>
@@ -16821,9 +16740,7 @@
       <c r="A49">
         <v>16</v>
       </c>
-      <c r="B49" s="60" t="s">
-        <v>49</v>
-      </c>
+      <c r="B49" s="60"/>
       <c r="C49" s="35"/>
       <c r="D49" s="36"/>
       <c r="E49" s="36"/>
@@ -16858,9 +16775,7 @@
       <c r="A50">
         <v>17</v>
       </c>
-      <c r="B50" s="60" t="s">
-        <v>50</v>
-      </c>
+      <c r="B50" s="60"/>
       <c r="C50" s="35"/>
       <c r="D50" s="36"/>
       <c r="E50" s="36"/>
@@ -16895,9 +16810,7 @@
       <c r="A51">
         <v>18</v>
       </c>
-      <c r="B51" s="60" t="s">
-        <v>51</v>
-      </c>
+      <c r="B51" s="60"/>
       <c r="C51" s="35"/>
       <c r="D51" s="36"/>
       <c r="E51" s="36"/>
@@ -16932,9 +16845,7 @@
       <c r="A52">
         <v>19</v>
       </c>
-      <c r="B52" s="60" t="s">
-        <v>52</v>
-      </c>
+      <c r="B52" s="60"/>
       <c r="C52" s="35"/>
       <c r="D52" s="36"/>
       <c r="E52" s="36"/>
@@ -16969,9 +16880,7 @@
       <c r="A53">
         <v>20</v>
       </c>
-      <c r="B53" s="60" t="s">
-        <v>53</v>
-      </c>
+      <c r="B53" s="60"/>
       <c r="C53" s="35"/>
       <c r="D53" s="36"/>
       <c r="E53" s="36"/>
@@ -17006,9 +16915,7 @@
       <c r="A54">
         <v>21</v>
       </c>
-      <c r="B54" s="60" t="s">
-        <v>54</v>
-      </c>
+      <c r="B54" s="60"/>
       <c r="C54" s="35"/>
       <c r="D54" s="36"/>
       <c r="E54" s="36"/>
@@ -17043,9 +16950,7 @@
       <c r="A55">
         <v>22</v>
       </c>
-      <c r="B55" s="60" t="s">
-        <v>55</v>
-      </c>
+      <c r="B55" s="60"/>
       <c r="C55" s="35"/>
       <c r="D55" s="36"/>
       <c r="E55" s="36"/>
@@ -17080,9 +16985,7 @@
       <c r="A56">
         <v>23</v>
       </c>
-      <c r="B56" s="61" t="s">
-        <v>56</v>
-      </c>
+      <c r="B56" s="61"/>
       <c r="C56" s="35"/>
       <c r="D56" s="36"/>
       <c r="E56" s="36"/>
@@ -17117,9 +17020,7 @@
       <c r="A57">
         <v>24</v>
       </c>
-      <c r="B57" s="34" t="s">
-        <v>57</v>
-      </c>
+      <c r="B57" s="34"/>
       <c r="C57" s="35"/>
       <c r="D57" s="36"/>
       <c r="E57" s="36"/>
@@ -17218,8 +17119,8 @@
       <c r="A60">
         <v>1</v>
       </c>
-      <c r="B60" s="42" t="s">
-        <v>75</v>
+      <c r="B60" s="101" t="s">
+        <v>37</v>
       </c>
       <c r="C60" s="35"/>
       <c r="D60" s="36"/>
@@ -17255,8 +17156,8 @@
       <c r="A61">
         <v>2</v>
       </c>
-      <c r="B61" s="42" t="s">
-        <v>76</v>
+      <c r="B61" s="101" t="s">
+        <v>99</v>
       </c>
       <c r="C61" s="35"/>
       <c r="D61" s="36"/>
@@ -17292,8 +17193,8 @@
       <c r="A62">
         <v>3</v>
       </c>
-      <c r="B62" s="65" t="s">
-        <v>77</v>
+      <c r="B62" s="101" t="s">
+        <v>59</v>
       </c>
       <c r="C62" s="35"/>
       <c r="D62" s="36"/>
@@ -17329,8 +17230,8 @@
       <c r="A63">
         <v>4</v>
       </c>
-      <c r="B63" s="60" t="s">
-        <v>78</v>
+      <c r="B63" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="C63" s="35"/>
       <c r="D63" s="36"/>
@@ -17366,8 +17267,8 @@
       <c r="A64">
         <v>5</v>
       </c>
-      <c r="B64" s="60" t="s">
-        <v>79</v>
+      <c r="B64" s="101" t="s">
+        <v>41</v>
       </c>
       <c r="C64" s="35"/>
       <c r="D64" s="36"/>
@@ -17403,8 +17304,8 @@
       <c r="A65">
         <v>6</v>
       </c>
-      <c r="B65" s="60" t="s">
-        <v>80</v>
+      <c r="B65" s="101" t="s">
+        <v>100</v>
       </c>
       <c r="C65" s="35"/>
       <c r="D65" s="36"/>
@@ -17440,8 +17341,8 @@
       <c r="A66">
         <v>7</v>
       </c>
-      <c r="B66" s="60" t="s">
-        <v>81</v>
+      <c r="B66" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="C66" s="35"/>
       <c r="D66" s="36"/>
@@ -17477,8 +17378,8 @@
       <c r="A67">
         <v>8</v>
       </c>
-      <c r="B67" s="60" t="s">
-        <v>82</v>
+      <c r="B67" s="101" t="s">
+        <v>40</v>
       </c>
       <c r="C67" s="35"/>
       <c r="D67" s="36"/>
@@ -17514,8 +17415,8 @@
       <c r="A68">
         <v>9</v>
       </c>
-      <c r="B68" s="60" t="s">
-        <v>83</v>
+      <c r="B68" s="101" t="s">
+        <v>16</v>
       </c>
       <c r="C68" s="35"/>
       <c r="D68" s="36"/>
@@ -17551,9 +17452,7 @@
       <c r="A69">
         <v>10</v>
       </c>
-      <c r="B69" s="42" t="s">
-        <v>84</v>
-      </c>
+      <c r="B69" s="42"/>
       <c r="C69" s="35"/>
       <c r="D69" s="36"/>
       <c r="E69" s="36"/>
@@ -17588,9 +17487,7 @@
       <c r="A70">
         <v>11</v>
       </c>
-      <c r="B70" s="42" t="s">
-        <v>85</v>
-      </c>
+      <c r="B70" s="42"/>
       <c r="C70" s="35"/>
       <c r="D70" s="36"/>
       <c r="E70" s="36"/>
@@ -17625,9 +17522,7 @@
       <c r="A71">
         <v>12</v>
       </c>
-      <c r="B71" s="42" t="s">
-        <v>86</v>
-      </c>
+      <c r="B71" s="42"/>
       <c r="C71" s="35"/>
       <c r="D71" s="36"/>
       <c r="E71" s="36"/>
@@ -17662,9 +17557,7 @@
       <c r="A72">
         <v>13</v>
       </c>
-      <c r="B72" s="42" t="s">
-        <v>87</v>
-      </c>
+      <c r="B72" s="42"/>
       <c r="C72" s="35"/>
       <c r="D72" s="36"/>
       <c r="E72" s="36"/>
@@ -17699,9 +17592,7 @@
       <c r="A73">
         <v>14</v>
       </c>
-      <c r="B73" s="42" t="s">
-        <v>88</v>
-      </c>
+      <c r="B73" s="42"/>
       <c r="C73" s="35"/>
       <c r="D73" s="36"/>
       <c r="E73" s="36"/>
@@ -17736,9 +17627,7 @@
       <c r="A74">
         <v>15</v>
       </c>
-      <c r="B74" s="42" t="s">
-        <v>66</v>
-      </c>
+      <c r="B74" s="42"/>
       <c r="C74" s="35"/>
       <c r="D74" s="36"/>
       <c r="E74" s="36"/>
@@ -17773,9 +17662,7 @@
       <c r="A75">
         <v>16</v>
       </c>
-      <c r="B75" s="42" t="s">
-        <v>89</v>
-      </c>
+      <c r="B75" s="42"/>
       <c r="C75" s="35"/>
       <c r="D75" s="36"/>
       <c r="E75" s="36"/>
@@ -17810,9 +17697,7 @@
       <c r="A76">
         <v>17</v>
       </c>
-      <c r="B76" s="42" t="s">
-        <v>90</v>
-      </c>
+      <c r="B76" s="42"/>
       <c r="C76" s="35"/>
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
@@ -17847,9 +17732,7 @@
       <c r="A77">
         <v>18</v>
       </c>
-      <c r="B77" s="42" t="s">
-        <v>89</v>
-      </c>
+      <c r="B77" s="42"/>
       <c r="C77" s="35"/>
       <c r="D77" s="36"/>
       <c r="E77" s="36"/>
@@ -17884,9 +17767,7 @@
       <c r="A78">
         <v>19</v>
       </c>
-      <c r="B78" s="42" t="s">
-        <v>91</v>
-      </c>
+      <c r="B78" s="42"/>
       <c r="C78" s="35"/>
       <c r="D78" s="36"/>
       <c r="E78" s="36"/>
@@ -17921,9 +17802,7 @@
       <c r="A79">
         <v>20</v>
       </c>
-      <c r="B79" s="42" t="s">
-        <v>92</v>
-      </c>
+      <c r="B79" s="42"/>
       <c r="C79" s="35"/>
       <c r="D79" s="36"/>
       <c r="E79" s="36"/>
@@ -17958,9 +17837,7 @@
       <c r="A80">
         <v>21</v>
       </c>
-      <c r="B80" s="42" t="s">
-        <v>93</v>
-      </c>
+      <c r="B80" s="42"/>
       <c r="C80" s="35"/>
       <c r="D80" s="36"/>
       <c r="E80" s="36"/>
@@ -17995,9 +17872,7 @@
       <c r="A81">
         <v>22</v>
       </c>
-      <c r="B81" s="42" t="s">
-        <v>94</v>
-      </c>
+      <c r="B81" s="42"/>
       <c r="C81" s="35"/>
       <c r="D81" s="36"/>
       <c r="E81" s="36"/>
@@ -18032,9 +17907,7 @@
       <c r="A82">
         <v>23</v>
       </c>
-      <c r="B82" s="66" t="s">
-        <v>95</v>
-      </c>
+      <c r="B82" s="66"/>
       <c r="C82" s="35"/>
       <c r="D82" s="36"/>
       <c r="E82" s="36"/>
@@ -18165,8 +18038,8 @@
       <c r="A86">
         <v>1</v>
       </c>
-      <c r="B86" s="60" t="s">
-        <v>58</v>
+      <c r="B86" s="101" t="s">
+        <v>37</v>
       </c>
       <c r="C86" s="35"/>
       <c r="D86" s="36"/>
@@ -18202,8 +18075,8 @@
       <c r="A87">
         <v>2</v>
       </c>
-      <c r="B87" s="60" t="s">
-        <v>59</v>
+      <c r="B87" s="101" t="s">
+        <v>99</v>
       </c>
       <c r="C87" s="35"/>
       <c r="D87" s="36"/>
@@ -18239,8 +18112,8 @@
       <c r="A88">
         <v>3</v>
       </c>
-      <c r="B88" s="60" t="s">
-        <v>60</v>
+      <c r="B88" s="101" t="s">
+        <v>59</v>
       </c>
       <c r="C88" s="35"/>
       <c r="D88" s="36"/>
@@ -18276,8 +18149,8 @@
       <c r="A89">
         <v>4</v>
       </c>
-      <c r="B89" s="60" t="s">
-        <v>61</v>
+      <c r="B89" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="C89" s="35"/>
       <c r="D89" s="36"/>
@@ -18313,8 +18186,8 @@
       <c r="A90">
         <v>5</v>
       </c>
-      <c r="B90" s="60" t="s">
-        <v>62</v>
+      <c r="B90" s="101" t="s">
+        <v>41</v>
       </c>
       <c r="C90" s="35"/>
       <c r="D90" s="36"/>
@@ -18350,8 +18223,8 @@
       <c r="A91">
         <v>6</v>
       </c>
-      <c r="B91" s="60" t="s">
-        <v>45</v>
+      <c r="B91" s="101" t="s">
+        <v>100</v>
       </c>
       <c r="C91" s="35"/>
       <c r="D91" s="36"/>
@@ -18387,8 +18260,8 @@
       <c r="A92">
         <v>7</v>
       </c>
-      <c r="B92" s="60" t="s">
-        <v>63</v>
+      <c r="B92" s="101" t="s">
+        <v>38</v>
       </c>
       <c r="C92" s="35"/>
       <c r="D92" s="36"/>
@@ -18424,8 +18297,8 @@
       <c r="A93">
         <v>8</v>
       </c>
-      <c r="B93" s="60" t="s">
-        <v>64</v>
+      <c r="B93" s="101" t="s">
+        <v>40</v>
       </c>
       <c r="C93" s="35"/>
       <c r="D93" s="36"/>
@@ -18461,8 +18334,8 @@
       <c r="A94">
         <v>9</v>
       </c>
-      <c r="B94" s="60" t="s">
-        <v>27</v>
+      <c r="B94" s="101" t="s">
+        <v>16</v>
       </c>
       <c r="C94" s="35"/>
       <c r="D94" s="36"/>
@@ -18498,9 +18371,7 @@
       <c r="A95">
         <v>10</v>
       </c>
-      <c r="B95" s="60" t="s">
-        <v>65</v>
-      </c>
+      <c r="B95" s="60"/>
       <c r="C95" s="35"/>
       <c r="D95" s="36"/>
       <c r="E95" s="36"/>
@@ -18535,9 +18406,7 @@
       <c r="A96">
         <v>11</v>
       </c>
-      <c r="B96" s="60" t="s">
-        <v>29</v>
-      </c>
+      <c r="B96" s="60"/>
       <c r="C96" s="35"/>
       <c r="D96" s="36"/>
       <c r="E96" s="36"/>
@@ -18572,9 +18441,7 @@
       <c r="A97">
         <v>12</v>
       </c>
-      <c r="B97" s="60" t="s">
-        <v>66</v>
-      </c>
+      <c r="B97" s="60"/>
       <c r="C97" s="35"/>
       <c r="D97" s="36"/>
       <c r="E97" s="36"/>
@@ -18609,9 +18476,7 @@
       <c r="A98">
         <v>13</v>
       </c>
-      <c r="B98" s="60" t="s">
-        <v>67</v>
-      </c>
+      <c r="B98" s="60"/>
       <c r="C98" s="35"/>
       <c r="D98" s="36"/>
       <c r="E98" s="36"/>
@@ -18646,9 +18511,7 @@
       <c r="A99">
         <v>14</v>
       </c>
-      <c r="B99" s="60" t="s">
-        <v>47</v>
-      </c>
+      <c r="B99" s="60"/>
       <c r="C99" s="35"/>
       <c r="D99" s="36"/>
       <c r="E99" s="36"/>
@@ -18683,9 +18546,7 @@
       <c r="A100">
         <v>15</v>
       </c>
-      <c r="B100" s="60" t="s">
-        <v>68</v>
-      </c>
+      <c r="B100" s="60"/>
       <c r="C100" s="35"/>
       <c r="D100" s="36"/>
       <c r="E100" s="36"/>
@@ -18720,9 +18581,7 @@
       <c r="A101">
         <v>16</v>
       </c>
-      <c r="B101" s="60" t="s">
-        <v>69</v>
-      </c>
+      <c r="B101" s="60"/>
       <c r="C101" s="35"/>
       <c r="D101" s="36"/>
       <c r="E101" s="36"/>
@@ -18757,9 +18616,7 @@
       <c r="A102">
         <v>17</v>
       </c>
-      <c r="B102" s="60" t="s">
-        <v>70</v>
-      </c>
+      <c r="B102" s="60"/>
       <c r="C102" s="35"/>
       <c r="D102" s="36"/>
       <c r="E102" s="36"/>
@@ -18794,9 +18651,7 @@
       <c r="A103">
         <v>18</v>
       </c>
-      <c r="B103" s="60" t="s">
-        <v>71</v>
-      </c>
+      <c r="B103" s="60"/>
       <c r="C103" s="35"/>
       <c r="D103" s="36"/>
       <c r="E103" s="36"/>
@@ -18831,9 +18686,7 @@
       <c r="A104">
         <v>19</v>
       </c>
-      <c r="B104" s="60" t="s">
-        <v>52</v>
-      </c>
+      <c r="B104" s="60"/>
       <c r="C104" s="35"/>
       <c r="D104" s="36"/>
       <c r="E104" s="36"/>
@@ -18868,9 +18721,7 @@
       <c r="A105">
         <v>20</v>
       </c>
-      <c r="B105" s="60" t="s">
-        <v>72</v>
-      </c>
+      <c r="B105" s="60"/>
       <c r="C105" s="35"/>
       <c r="D105" s="36"/>
       <c r="E105" s="36"/>

</xml_diff>